<commit_message>
Update for 2021 preliminary elections
</commit_message>
<xml_diff>
--- a/file_index.xlsx
+++ b/file_index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sharon\My Documents Data Drive\R\FraminghamCityData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EED5EF6-B4DA-487A-AE9E-007EA86EC6A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA06317D-F8C1-41AE-95AF-DCC68DEA88AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12375" yWindow="1425" windowWidth="22245" windowHeight="13410" xr2:uid="{0B152F85-AA73-4361-9908-3A1D4A4A333B}"/>
+    <workbookView xWindow="13455" yWindow="630" windowWidth="26010" windowHeight="14610" xr2:uid="{0B152F85-AA73-4361-9908-3A1D4A4A333B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>File</t>
   </si>
@@ -172,6 +172,21 @@
   </si>
   <si>
     <t>data/elections/2020_us_senate_democratic_primary.csv</t>
+  </si>
+  <si>
+    <t>data-raw/elections/Official Results September 14, 2021.pdf</t>
+  </si>
+  <si>
+    <t>data-raw/elections/Official Results September 14, 2021.xlsx</t>
+  </si>
+  <si>
+    <t>data/elections/2021_preliminary_turnout_bydistrict_framingham.csv</t>
+  </si>
+  <si>
+    <t>data/elections/tidy/2021_preliminary_turnout_tidy.csv</t>
+  </si>
+  <si>
+    <t>data/elections/2021_preliminary_turnout.csv</t>
   </si>
 </sst>
 </file>
@@ -532,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93CD3FA-8F18-47FA-8624-3C927A87969A}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +788,31 @@
         <v>44</v>
       </c>
     </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>